<commit_message>
Remit ID Report first try
</commit_message>
<xml_diff>
--- a/ECI097_99_Dispute Report-2020-06-29.xlsx
+++ b/ECI097_99_Dispute Report-2020-06-29.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\my_reports\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02DBF20-795E-4D54-959E-E9EA87989833}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -58,8 +64,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,15 +138,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -149,6 +156,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -157,19 +172,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>809625</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>52673</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1074421</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>158697</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png"/>
+        <xdr:cNvPr id="2" name="Picture 1" descr="logo.png">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -182,8 +203,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="3238500" cy="1386173"/>
+          <a:off x="1" y="0"/>
+          <a:ext cx="2217420" cy="905457"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -238,7 +259,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -270,9 +291,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -304,6 +343,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -479,94 +536,94 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.7109375" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" customWidth="1"/>
-    <col min="5" max="5" width="25.7109375" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="40.7109375" customWidth="1"/>
-    <col min="10" max="10" width="40.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="30.6640625" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="25.6640625" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="10" width="40.6640625" customWidth="1"/>
+    <col min="11" max="11" width="30.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
-      <c r="A1"/>
-      <c r="B1"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2"/>
-      <c r="B2"/>
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:11">
-      <c r="A3"/>
-      <c r="B3"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:11">
-      <c r="A4"/>
-      <c r="B4"/>
-      <c r="D4" s="2" t="s">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:11">
-      <c r="A5"/>
-      <c r="B5"/>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
     </row>
-    <row r="7" spans="1:11">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="K7" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>